<commit_message>
Casi listo, con ponderaciones y todo
</commit_message>
<xml_diff>
--- a/etf_dfs/EDEN.xlsx
+++ b/etf_dfs/EDEN.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Open</t>
   </si>
@@ -37,7 +37,10 @@
     <t>Return</t>
   </si>
   <si>
-    <t>Return_12</t>
+    <t>Volatility</t>
+  </si>
+  <si>
+    <t>Trend</t>
   </si>
   <si>
     <t>EDEN</t>
@@ -404,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +441,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>40909</v>
       </c>
@@ -456,13 +462,13 @@
         <v>26.35000038146973</v>
       </c>
       <c r="F2">
-        <v>23.26592826843262</v>
+        <v>23.26592063903809</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>40940</v>
       </c>
@@ -488,7 +494,7 @@
         <v>0.1252371608837328</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>40969</v>
       </c>
@@ -505,7 +511,7 @@
         <v>29.44000053405762</v>
       </c>
       <c r="F4">
-        <v>25.99426078796387</v>
+        <v>25.99425888061523</v>
       </c>
       <c r="G4">
         <v>9100</v>
@@ -513,8 +519,11 @@
       <c r="H4">
         <v>-0.007082599904703279</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="I4">
+        <v>0.093564200138485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>41000</v>
       </c>
@@ -539,8 +548,11 @@
       <c r="H5">
         <v>0.0129075799549323</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5">
+        <v>0.07132795283941339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>41030</v>
       </c>
@@ -565,8 +577,11 @@
       <c r="H6">
         <v>-0.09121392827601527</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="I6">
+        <v>0.08911439465925221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>41061</v>
       </c>
@@ -583,7 +598,7 @@
         <v>27.26000022888184</v>
       </c>
       <c r="F7">
-        <v>24.3504524230957</v>
+        <v>24.3504467010498</v>
       </c>
       <c r="G7">
         <v>3700</v>
@@ -591,8 +606,11 @@
       <c r="H7">
         <v>0.005904053326933223</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="I7">
+        <v>0.07719666426828323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>41091</v>
       </c>
@@ -609,7 +627,7 @@
         <v>27.8799991607666</v>
       </c>
       <c r="F8">
-        <v>24.90427207946777</v>
+        <v>24.90427017211914</v>
       </c>
       <c r="G8">
         <v>2000</v>
@@ -617,8 +635,11 @@
       <c r="H8">
         <v>0.02274390780187452</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="I8">
+        <v>0.0692694520020858</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>41122</v>
       </c>
@@ -635,7 +656,7 @@
         <v>29.1200008392334</v>
       </c>
       <c r="F9">
-        <v>26.01192855834961</v>
+        <v>26.01192283630371</v>
       </c>
       <c r="G9">
         <v>31800</v>
@@ -643,8 +664,11 @@
       <c r="H9">
         <v>0.04447638865828085</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="I9">
+        <v>0.06445687347845433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>41153</v>
       </c>
@@ -661,7 +685,7 @@
         <v>30.27000045776367</v>
       </c>
       <c r="F10">
-        <v>27.03917694091797</v>
+        <v>27.03918647766113</v>
       </c>
       <c r="G10">
         <v>18900</v>
@@ -669,8 +693,11 @@
       <c r="H10">
         <v>0.03949174400369104</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="I10">
+        <v>0.06024392750331733</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>41183</v>
       </c>
@@ -687,7 +714,7 @@
         <v>30.27000045776367</v>
       </c>
       <c r="F11">
-        <v>27.03917694091797</v>
+        <v>27.03918647766113</v>
       </c>
       <c r="G11">
         <v>2000</v>
@@ -695,8 +722,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="I11">
+        <v>0.05670997255250021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>41214</v>
       </c>
@@ -713,7 +743,7 @@
         <v>30.71999931335449</v>
       </c>
       <c r="F12">
-        <v>27.44114685058594</v>
+        <v>27.44115447998047</v>
       </c>
       <c r="G12">
         <v>5100</v>
@@ -721,8 +751,11 @@
       <c r="H12">
         <v>0.01486616613100855</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="I12">
+        <v>0.05347069850742251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>41244</v>
       </c>
@@ -739,7 +772,7 @@
         <v>31.97999954223633</v>
       </c>
       <c r="F13">
-        <v>28.56666374206543</v>
+        <v>28.56666564941406</v>
       </c>
       <c r="G13">
         <v>3800</v>
@@ -747,8 +780,11 @@
       <c r="H13">
         <v>0.04101563336735148</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="I13">
+        <v>0.05125239543580462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>41275</v>
       </c>
@@ -765,7 +801,7 @@
         <v>34.81000137329102</v>
       </c>
       <c r="F14">
-        <v>31.09461975097656</v>
+        <v>31.09460830688477</v>
       </c>
       <c r="G14">
         <v>600</v>
@@ -774,13 +810,16 @@
         <v>0.08849286652793964</v>
       </c>
       <c r="I14">
-        <v>0.3210626515880686</v>
+        <v>0.05283118690159319</v>
       </c>
       <c r="J14">
         <v>0.3210626515880686</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>0.3210626515880686</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>41306</v>
       </c>
@@ -797,7 +836,7 @@
         <v>34.72999954223633</v>
       </c>
       <c r="F15">
-        <v>31.02314758300781</v>
+        <v>31.02314186096191</v>
       </c>
       <c r="G15">
         <v>56800</v>
@@ -806,13 +845,16 @@
         <v>-0.002298242685967566</v>
       </c>
       <c r="I15">
-        <v>0.1713322087374065</v>
+        <v>0.0511347382158598</v>
       </c>
       <c r="J15">
         <v>0.1713322087374065</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>0.1713322087374065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>41334</v>
       </c>
@@ -829,7 +871,7 @@
         <v>34.56000137329102</v>
       </c>
       <c r="F16">
-        <v>30.87129783630371</v>
+        <v>30.87129211425781</v>
       </c>
       <c r="G16">
         <v>7400</v>
@@ -838,13 +880,16 @@
         <v>-0.004894850883558788</v>
       </c>
       <c r="I16">
-        <v>0.1739130688299524</v>
+        <v>0.04967743575642662</v>
       </c>
       <c r="J16">
         <v>0.1739130688299524</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>0.1739130688299524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
         <v>41365</v>
       </c>
@@ -870,13 +915,16 @@
         <v>0.03674769697043945</v>
       </c>
       <c r="I17">
-        <v>0.2015426625666132</v>
+        <v>0.04804960903249037</v>
       </c>
       <c r="J17">
         <v>0.2015426625666132</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>0.2015426625666132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
         <v>41395</v>
       </c>
@@ -893,7 +941,7 @@
         <v>35.90999984741211</v>
       </c>
       <c r="F18">
-        <v>32.07719802856445</v>
+        <v>32.07720947265625</v>
       </c>
       <c r="G18">
         <v>25300</v>
@@ -902,13 +950,16 @@
         <v>0.00223271036196504</v>
       </c>
       <c r="I18">
-        <v>0.3250922266394665</v>
+        <v>0.04667631531049968</v>
       </c>
       <c r="J18">
         <v>0.3250922266394665</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>0.3250922266394665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
         <v>41426</v>
       </c>
@@ -925,7 +976,7 @@
         <v>34.29999923706055</v>
       </c>
       <c r="F19">
-        <v>30.6390438079834</v>
+        <v>30.63904762268066</v>
       </c>
       <c r="G19">
         <v>8700</v>
@@ -934,13 +985,16 @@
         <v>-0.04483432517941344</v>
       </c>
       <c r="I19">
-        <v>0.2582538132453818</v>
+        <v>0.04789472370680067</v>
       </c>
       <c r="J19">
         <v>0.2582538132453818</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>0.2582538132453818</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
         <v>41456</v>
       </c>
@@ -957,7 +1011,7 @@
         <v>37.43000030517578</v>
       </c>
       <c r="F20">
-        <v>33.43496322631836</v>
+        <v>33.43497085571289</v>
       </c>
       <c r="G20">
         <v>700</v>
@@ -966,13 +1020,16 @@
         <v>0.09125367748502233</v>
       </c>
       <c r="I20">
-        <v>0.3425395061649847</v>
+        <v>0.04967709086278745</v>
       </c>
       <c r="J20">
         <v>0.3425395061649847</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>0.3425395061649847</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="2">
         <v>41487</v>
       </c>
@@ -989,7 +1046,7 @@
         <v>37.68999862670898</v>
       </c>
       <c r="F21">
-        <v>33.66721725463867</v>
+        <v>33.66722106933594</v>
       </c>
       <c r="G21">
         <v>800</v>
@@ -998,13 +1055,16 @@
         <v>0.006946254860095591</v>
       </c>
       <c r="I21">
-        <v>0.2942993660882463</v>
+        <v>0.04838250067088842</v>
       </c>
       <c r="J21">
         <v>0.2942993660882463</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>0.2942993660882463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="2">
         <v>41518</v>
       </c>
@@ -1021,7 +1081,7 @@
         <v>40.45000076293945</v>
       </c>
       <c r="F22">
-        <v>36.13264465332031</v>
+        <v>36.13264083862305</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1030,13 +1090,16 @@
         <v>0.07322903254962165</v>
       </c>
       <c r="I22">
-        <v>0.3363065791617723</v>
+        <v>0.04856718942117204</v>
       </c>
       <c r="J22">
         <v>0.3363065791617723</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>0.3363065791617723</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="2">
         <v>41548</v>
       </c>
@@ -1053,7 +1116,7 @@
         <v>41.70999908447266</v>
       </c>
       <c r="F23">
-        <v>37.25815582275391</v>
+        <v>37.25814437866211</v>
       </c>
       <c r="G23">
         <v>31800</v>
@@ -1062,13 +1125,16 @@
         <v>0.03114952528474668</v>
       </c>
       <c r="I23">
-        <v>0.3779318947375452</v>
+        <v>0.04737282009094167</v>
       </c>
       <c r="J23">
         <v>0.3779318947375452</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>0.3779318947375452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="2">
         <v>41579</v>
       </c>
@@ -1085,7 +1151,7 @@
         <v>43.22999954223633</v>
       </c>
       <c r="F24">
-        <v>38.61591720581055</v>
+        <v>38.61591339111328</v>
       </c>
       <c r="G24">
         <v>2100</v>
@@ -1094,13 +1160,16 @@
         <v>0.036442111990588</v>
       </c>
       <c r="I24">
-        <v>0.407226579052804</v>
+        <v>0.04631777644252788</v>
       </c>
       <c r="J24">
         <v>0.407226579052804</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>0.407226579052804</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="2">
         <v>41609</v>
       </c>
@@ -1117,7 +1186,7 @@
         <v>45</v>
       </c>
       <c r="F25">
-        <v>40.21220397949219</v>
+        <v>40.21219253540039</v>
       </c>
       <c r="G25">
         <v>4300</v>
@@ -1126,13 +1195,16 @@
         <v>0.04094380005797493</v>
       </c>
       <c r="I25">
-        <v>0.4071294760516808</v>
+        <v>0.04539441846192326</v>
       </c>
       <c r="J25">
         <v>0.4071294760516808</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>0.4071294760516808</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="2">
         <v>41640</v>
       </c>
@@ -1149,7 +1221,7 @@
         <v>45.68000030517578</v>
       </c>
       <c r="F26">
-        <v>40.81984329223633</v>
+        <v>40.81984710693359</v>
       </c>
       <c r="G26">
         <v>2900</v>
@@ -1158,13 +1230,16 @@
         <v>0.01511111789279518</v>
       </c>
       <c r="I26">
-        <v>0.3122665470569355</v>
+        <v>0.04443806136380691</v>
       </c>
       <c r="J26">
         <v>0.3122665470569355</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>0.3122665470569355</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="2">
         <v>41671</v>
       </c>
@@ -1181,7 +1256,7 @@
         <v>50.9900016784668</v>
       </c>
       <c r="F27">
-        <v>45.56489181518555</v>
+        <v>45.56488800048828</v>
       </c>
       <c r="G27">
         <v>5200</v>
@@ -1190,13 +1265,16 @@
         <v>0.1162434618611279</v>
       </c>
       <c r="I27">
-        <v>0.4681831946601707</v>
+        <v>0.04724334390837787</v>
       </c>
       <c r="J27">
         <v>0.4681831946601707</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>0.4681831946601707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="2">
         <v>41699</v>
       </c>
@@ -1213,7 +1291,7 @@
         <v>49.58000183105469</v>
       </c>
       <c r="F28">
-        <v>44.30490875244141</v>
+        <v>44.30490112304688</v>
       </c>
       <c r="G28">
         <v>6100</v>
@@ -1222,13 +1300,16 @@
         <v>-0.02765247697584516</v>
       </c>
       <c r="I28">
-        <v>0.4346064774572482</v>
+        <v>0.04754937944962202</v>
       </c>
       <c r="J28">
         <v>0.4346064774572482</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>0.4346064774572482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="2">
         <v>41730</v>
       </c>
@@ -1245,7 +1326,7 @@
         <v>50.90000152587891</v>
       </c>
       <c r="F29">
-        <v>45.48446655273438</v>
+        <v>45.48446273803711</v>
       </c>
       <c r="G29">
         <v>22500</v>
@@ -1254,13 +1335,16 @@
         <v>0.02662363142547175</v>
       </c>
       <c r="I29">
-        <v>0.42059723485034</v>
+        <v>0.04662636270103054</v>
       </c>
       <c r="J29">
         <v>0.42059723485034</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>0.42059723485034</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="2">
         <v>41760</v>
       </c>
@@ -1277,7 +1361,7 @@
         <v>52.65000152587891</v>
       </c>
       <c r="F30">
-        <v>47.04827499389648</v>
+        <v>47.04827117919922</v>
       </c>
       <c r="G30">
         <v>9200</v>
@@ -1286,13 +1370,16 @@
         <v>0.03438113845851754</v>
       </c>
       <c r="I30">
-        <v>0.4661654622555835</v>
+        <v>0.0457841222496381</v>
       </c>
       <c r="J30">
         <v>0.4661654622555835</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>0.4661654622555835</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="2">
         <v>41791</v>
       </c>
@@ -1309,7 +1396,7 @@
         <v>53.15000152587891</v>
       </c>
       <c r="F31">
-        <v>47.8586311340332</v>
+        <v>47.85863876342773</v>
       </c>
       <c r="G31">
         <v>12100</v>
@@ -1318,13 +1405,16 @@
         <v>0.009496675888114314</v>
       </c>
       <c r="I31">
-        <v>0.5495627611691392</v>
+        <v>0.04506365079700764</v>
       </c>
       <c r="J31">
         <v>0.5495627611691392</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>0.5495627611691392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="2">
         <v>41821</v>
       </c>
@@ -1341,7 +1431,7 @@
         <v>51.34000015258789</v>
       </c>
       <c r="F32">
-        <v>46.22883605957031</v>
+        <v>46.22883987426758</v>
       </c>
       <c r="G32">
         <v>28700</v>
@@ -1350,13 +1440,16 @@
         <v>-0.03405458741915035</v>
       </c>
       <c r="I32">
-        <v>0.3716270300294027</v>
+        <v>0.04559299911228007</v>
       </c>
       <c r="J32">
         <v>0.3716270300294027</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <v>0.3716270300294027</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="2">
         <v>41852</v>
       </c>
@@ -1373,7 +1466,7 @@
         <v>50.58000183105469</v>
       </c>
       <c r="F33">
-        <v>45.54449462890625</v>
+        <v>45.54449844360352</v>
       </c>
       <c r="G33">
         <v>51300</v>
@@ -1382,13 +1475,16 @@
         <v>-0.0148032395651424</v>
       </c>
       <c r="I33">
-        <v>0.3420006281244918</v>
+        <v>0.04535049898619727</v>
       </c>
       <c r="J33">
         <v>0.3420006281244918</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <v>0.3420006281244918</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="2">
         <v>41883</v>
       </c>
@@ -1414,13 +1510,16 @@
         <v>-0.03202852289316038</v>
       </c>
       <c r="I34">
-        <v>0.2103831436594217</v>
+        <v>0.04563244664400216</v>
       </c>
       <c r="J34">
         <v>0.2103831436594217</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34">
+        <v>0.2103831436594217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="2">
         <v>41913</v>
       </c>
@@ -1437,7 +1536,7 @@
         <v>49.27999877929688</v>
       </c>
       <c r="F35">
-        <v>44.37390899658203</v>
+        <v>44.3739128112793</v>
       </c>
       <c r="G35">
         <v>256500</v>
@@ -1446,13 +1545,16 @@
         <v>0.00653594160147164</v>
       </c>
       <c r="I35">
-        <v>0.1814912457680273</v>
+        <v>0.04497982930991846</v>
       </c>
       <c r="J35">
         <v>0.1814912457680273</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35">
+        <v>0.1814912457680273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="2">
         <v>41944</v>
       </c>
@@ -1469,7 +1571,7 @@
         <v>49.02999877929688</v>
       </c>
       <c r="F36">
-        <v>44.1488037109375</v>
+        <v>44.1487922668457</v>
       </c>
       <c r="G36">
         <v>10800</v>
@@ -1478,13 +1580,16 @@
         <v>-0.005073052073715334</v>
       </c>
       <c r="I36">
-        <v>0.1341660721368703</v>
+        <v>0.0445031237068035</v>
       </c>
       <c r="J36">
         <v>0.1341660721368703</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36">
+        <v>0.1341660721368703</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="2">
         <v>41974</v>
       </c>
@@ -1510,13 +1615,16 @@
         <v>-0.04160712118335752</v>
       </c>
       <c r="I37">
-        <v>0.04422225952148429</v>
+        <v>0.04503895296619311</v>
       </c>
       <c r="J37">
         <v>0.04422225952148429</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37">
+        <v>0.04422225952148429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="2">
         <v>42005</v>
       </c>
@@ -1533,7 +1641,7 @@
         <v>47.31999969482422</v>
       </c>
       <c r="F38">
-        <v>42.614501953125</v>
+        <v>42.61450958251953</v>
       </c>
       <c r="G38">
         <v>37900</v>
@@ -1542,13 +1650,16 @@
         <v>0.007022728337305884</v>
       </c>
       <c r="I38">
-        <v>0.03590191284352118</v>
+        <v>0.04442604300086098</v>
       </c>
       <c r="J38">
         <v>0.03590191284352118</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38">
+        <v>0.03590191284352118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="2">
         <v>42036</v>
       </c>
@@ -1574,13 +1685,16 @@
         <v>0.07840234802196022</v>
       </c>
       <c r="I39">
-        <v>0.000784410659216972</v>
+        <v>0.04494050169677528</v>
       </c>
       <c r="J39">
         <v>0.000784410659216972</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39">
+        <v>0.000784410659216972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="2">
         <v>42064</v>
       </c>
@@ -1606,13 +1720,16 @@
         <v>0.02880660897251497</v>
       </c>
       <c r="I40">
-        <v>0.05889467650475866</v>
+        <v>0.0443576756061458</v>
       </c>
       <c r="J40">
         <v>0.05889467650475866</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40">
+        <v>0.05889467650475866</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="2">
         <v>42095</v>
       </c>
@@ -1629,7 +1746,7 @@
         <v>55.15000152587891</v>
       </c>
       <c r="F41">
-        <v>49.66589736938477</v>
+        <v>49.66590118408203</v>
       </c>
       <c r="G41">
         <v>13300</v>
@@ -1638,13 +1755,16 @@
         <v>0.05047621954055059</v>
       </c>
       <c r="I41">
-        <v>0.0834970505421142</v>
+        <v>0.04405497253070396</v>
       </c>
       <c r="J41">
         <v>0.0834970505421142</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41">
+        <v>0.0834970505421142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="2">
         <v>42125</v>
       </c>
@@ -1670,13 +1790,16 @@
         <v>0.007615560422935541</v>
       </c>
       <c r="I42">
-        <v>0.05546055240872216</v>
+        <v>0.04353086099310136</v>
       </c>
       <c r="J42">
         <v>0.05546055240872216</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42">
+        <v>0.05546055240872216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="2">
         <v>42156</v>
       </c>
@@ -1702,13 +1825,16 @@
         <v>-0.03185172696570182</v>
       </c>
       <c r="I43">
-        <v>0.01222949562598141</v>
+        <v>0.04373168513607511</v>
       </c>
       <c r="J43">
         <v>0.01222949562598141</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43">
+        <v>0.01222949562598141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="2">
         <v>42186</v>
       </c>
@@ -1725,7 +1851,7 @@
         <v>56.43000030517578</v>
       </c>
       <c r="F44">
-        <v>51.5699348449707</v>
+        <v>51.56993865966797</v>
       </c>
       <c r="G44">
         <v>15900</v>
@@ -1734,13 +1860,16 @@
         <v>0.04888477891099186</v>
       </c>
       <c r="I44">
-        <v>0.09914297112309844</v>
+        <v>0.04344922889129261</v>
       </c>
       <c r="J44">
         <v>0.09914297112309844</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44">
+        <v>0.09914297112309844</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="2">
         <v>42217</v>
       </c>
@@ -1757,7 +1886,7 @@
         <v>53.97999954223633</v>
       </c>
       <c r="F45">
-        <v>49.33094787597656</v>
+        <v>49.3309440612793</v>
       </c>
       <c r="G45">
         <v>8000</v>
@@ -1766,13 +1895,16 @@
         <v>-0.04341663564929554</v>
       </c>
       <c r="I45">
-        <v>0.06722019747128871</v>
+        <v>0.04397796616972521</v>
       </c>
       <c r="J45">
         <v>0.06722019747128871</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45">
+        <v>0.06722019747128871</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="2">
         <v>42248</v>
       </c>
@@ -1789,7 +1921,7 @@
         <v>53.04000091552734</v>
       </c>
       <c r="F46">
-        <v>48.47190856933594</v>
+        <v>48.47190475463867</v>
       </c>
       <c r="G46">
         <v>34200</v>
@@ -1798,13 +1930,16 @@
         <v>-0.01741383169100419</v>
       </c>
       <c r="I46">
-        <v>0.08333337229061821</v>
+        <v>0.04378551520455536</v>
       </c>
       <c r="J46">
         <v>0.08333337229061821</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46">
+        <v>0.08333337229061821</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="2">
         <v>42278</v>
       </c>
@@ -1821,7 +1956,7 @@
         <v>52.97999954223633</v>
       </c>
       <c r="F47">
-        <v>48.41706848144531</v>
+        <v>48.41706466674805</v>
       </c>
       <c r="G47">
         <v>8700</v>
@@ -1830,13 +1965,16 @@
         <v>-0.001131247591540818</v>
       </c>
       <c r="I47">
-        <v>0.07508118617271298</v>
+        <v>0.04336886115420008</v>
       </c>
       <c r="J47">
         <v>0.07508118617271298</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47">
+        <v>0.07508118617271298</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="2">
         <v>42309</v>
       </c>
@@ -1862,13 +2000,16 @@
         <v>0.04058138060505079</v>
       </c>
       <c r="I48">
-        <v>0.1244136740911792</v>
+        <v>0.04303052017245091</v>
       </c>
       <c r="J48">
         <v>0.1244136740911792</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48">
+        <v>0.1244136740911792</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="2">
         <v>42339</v>
       </c>
@@ -1885,7 +2026,7 @@
         <v>55.84999847412109</v>
       </c>
       <c r="F49">
-        <v>51.04924011230469</v>
+        <v>51.04923248291016</v>
       </c>
       <c r="G49">
         <v>17600</v>
@@ -1894,13 +2035,16 @@
         <v>0.01305999260033164</v>
       </c>
       <c r="I49">
-        <v>0.1885506805528461</v>
+        <v>0.04256423263586444</v>
       </c>
       <c r="J49">
         <v>0.1885506805528461</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49">
+        <v>0.1885506805528461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="2">
         <v>42370</v>
       </c>
@@ -1917,7 +2061,7 @@
         <v>54.11999893188477</v>
       </c>
       <c r="F50">
-        <v>49.46793746948242</v>
+        <v>49.46794128417969</v>
       </c>
       <c r="G50">
         <v>15300</v>
@@ -1926,13 +2070,16 @@
         <v>-0.03097582076099692</v>
       </c>
       <c r="I50">
-        <v>0.1437024361985428</v>
+        <v>0.0426740490294507</v>
       </c>
       <c r="J50">
         <v>0.1437024361985428</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50">
+        <v>0.1437024361985428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="2">
         <v>42401</v>
       </c>
@@ -1958,13 +2105,16 @@
         <v>-0.02254245066673677</v>
       </c>
       <c r="I51">
-        <v>0.03664516541867324</v>
+        <v>0.04258425825417343</v>
       </c>
       <c r="J51">
         <v>0.03664516541867324</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51">
+        <v>0.03664516541867324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="2">
         <v>42430</v>
       </c>
@@ -1981,7 +2131,7 @@
         <v>56.52000045776367</v>
       </c>
       <c r="F52">
-        <v>51.66164398193359</v>
+        <v>51.66165161132812</v>
       </c>
       <c r="G52">
         <v>159400</v>
@@ -1990,13 +2140,16 @@
         <v>0.06843097972528134</v>
       </c>
       <c r="I52">
-        <v>0.07657143729073668</v>
+        <v>0.04281467707586233</v>
       </c>
       <c r="J52">
         <v>0.07657143729073668</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52">
+        <v>0.07657143729073668</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="2">
         <v>42461</v>
       </c>
@@ -2013,7 +2166,7 @@
         <v>57.25</v>
       </c>
       <c r="F53">
-        <v>52.32889175415039</v>
+        <v>52.32889938354492</v>
       </c>
       <c r="G53">
         <v>13600</v>
@@ -2022,13 +2175,16 @@
         <v>0.01291577382031073</v>
       </c>
       <c r="I53">
-        <v>0.03807794045364954</v>
+        <v>0.04238695098118451</v>
       </c>
       <c r="J53">
         <v>0.03807794045364954</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53">
+        <v>0.03807794045364954</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="2">
         <v>42491</v>
       </c>
@@ -2054,13 +2210,16 @@
         <v>0.02323147303152284</v>
       </c>
       <c r="I54">
-        <v>0.05416595560123461</v>
+        <v>0.04198068681802958</v>
       </c>
       <c r="J54">
         <v>0.05416595560123461</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54">
+        <v>0.05416595560123461</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="2">
         <v>42522</v>
       </c>
@@ -2077,7 +2236,7 @@
         <v>55.36000061035156</v>
       </c>
       <c r="F55">
-        <v>51.17135620117188</v>
+        <v>51.17136001586914</v>
       </c>
       <c r="G55">
         <v>40400</v>
@@ -2086,13 +2245,16 @@
         <v>-0.05496758484217257</v>
       </c>
       <c r="I55">
-        <v>0.02899630846493384</v>
+        <v>0.04271289501003216</v>
       </c>
       <c r="J55">
         <v>0.02899630846493384</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55">
+        <v>0.02899630846493384</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="2">
         <v>42552</v>
       </c>
@@ -2109,7 +2271,7 @@
         <v>57.2400016784668</v>
       </c>
       <c r="F56">
-        <v>52.90911102294922</v>
+        <v>52.90911483764648</v>
       </c>
       <c r="G56">
         <v>8600</v>
@@ -2118,13 +2280,16 @@
         <v>0.03395955649183469</v>
       </c>
       <c r="I56">
-        <v>0.01435409124420506</v>
+        <v>0.04238676874127449</v>
       </c>
       <c r="J56">
         <v>0.01435409124420506</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56">
+        <v>0.01435409124420506</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="2">
         <v>42583</v>
       </c>
@@ -2141,7 +2306,7 @@
         <v>56.36000061035156</v>
       </c>
       <c r="F57">
-        <v>52.0956916809082</v>
+        <v>52.09569931030273</v>
       </c>
       <c r="G57">
         <v>7500</v>
@@ -2150,13 +2315,16 @@
         <v>-0.01537388263994899</v>
       </c>
       <c r="I57">
-        <v>0.04409042401441687</v>
+        <v>0.04219610984560418</v>
       </c>
       <c r="J57">
         <v>0.04409042401441687</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57">
+        <v>0.04409042401441687</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="2">
         <v>42614</v>
       </c>
@@ -2173,7 +2341,7 @@
         <v>55.52999877929688</v>
       </c>
       <c r="F58">
-        <v>51.32849884033203</v>
+        <v>51.3284912109375</v>
       </c>
       <c r="G58">
         <v>18000</v>
@@ -2182,13 +2350,16 @@
         <v>-0.0147267888940058</v>
       </c>
       <c r="I58">
-        <v>0.04694566027129521</v>
+        <v>0.04199620417460621</v>
       </c>
       <c r="J58">
         <v>0.04694566027129521</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58">
+        <v>0.04694566027129521</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="2">
         <v>42644</v>
       </c>
@@ -2214,13 +2385,16 @@
         <v>-0.04790203324124387</v>
       </c>
       <c r="I59">
-        <v>-0.002076266728992082</v>
+        <v>0.04242585718705426</v>
       </c>
       <c r="J59">
         <v>-0.002076266728992082</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59">
+        <v>-0.002076266728992082</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="2">
         <v>42675</v>
       </c>
@@ -2237,7 +2411,7 @@
         <v>48.88999938964844</v>
       </c>
       <c r="F60">
-        <v>45.19088745117188</v>
+        <v>45.19089126586914</v>
       </c>
       <c r="G60">
         <v>64300</v>
@@ -2246,13 +2420,16 @@
         <v>-0.07527897905509651</v>
       </c>
       <c r="I60">
-        <v>-0.113187040768547</v>
+        <v>0.04362593534764143</v>
       </c>
       <c r="J60">
         <v>-0.113187040768547</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60">
+        <v>-0.113187040768547</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="2">
         <v>42705</v>
       </c>
@@ -2269,7 +2446,7 @@
         <v>50.9900016784668</v>
       </c>
       <c r="F61">
-        <v>47.16225051879883</v>
+        <v>47.16223907470703</v>
       </c>
       <c r="G61">
         <v>19300</v>
@@ -2278,13 +2455,16 @@
         <v>0.04295361658897856</v>
       </c>
       <c r="I61">
-        <v>-0.08701874536140308</v>
+        <v>0.04344000986857272</v>
       </c>
       <c r="J61">
         <v>-0.08701874536140308</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61">
+        <v>-0.08701874536140308</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="2">
         <v>42736</v>
       </c>
@@ -2301,7 +2481,7 @@
         <v>53.88000106811523</v>
       </c>
       <c r="F62">
-        <v>49.83529281616211</v>
+        <v>49.83529663085938</v>
       </c>
       <c r="G62">
         <v>24400</v>
@@ -2310,13 +2490,16 @@
         <v>0.05667776612113529</v>
       </c>
       <c r="I62">
-        <v>-0.004434550415856275</v>
+        <v>0.04345198586896835</v>
       </c>
       <c r="J62">
         <v>-0.004434550415856275</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="K62">
+        <v>-0.004434550415856275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="2">
         <v>42767</v>
       </c>
@@ -2342,13 +2525,16 @@
         <v>-0.00668152567214042</v>
       </c>
       <c r="I63">
-        <v>0.01172020631382131</v>
+        <v>0.04316128966489189</v>
       </c>
       <c r="J63">
         <v>0.01172020631382131</v>
       </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="K63">
+        <v>0.01172020631382131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="2">
         <v>42795</v>
       </c>
@@ -2365,7 +2551,7 @@
         <v>55.40000152587891</v>
       </c>
       <c r="F64">
-        <v>51.24119186401367</v>
+        <v>51.24118804931641</v>
       </c>
       <c r="G64">
         <v>14000</v>
@@ -2374,13 +2560,16 @@
         <v>0.03512707496329104</v>
       </c>
       <c r="I64">
-        <v>-0.01981597527979007</v>
+        <v>0.04290167262318924</v>
       </c>
       <c r="J64">
         <v>-0.01981597527979007</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="K64">
+        <v>-0.01981597527979007</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="2">
         <v>42826</v>
       </c>
@@ -2397,7 +2586,7 @@
         <v>59.4900016784668</v>
       </c>
       <c r="F65">
-        <v>55.02416229248047</v>
+        <v>55.0241584777832</v>
       </c>
       <c r="G65">
         <v>27500</v>
@@ -2406,13 +2595,16 @@
         <v>0.07382671552233333</v>
       </c>
       <c r="I65">
-        <v>0.03912666687278255</v>
+        <v>0.0432399685553312</v>
       </c>
       <c r="J65">
         <v>0.03912666687278255</v>
       </c>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="K65">
+        <v>0.03912666687278255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="2">
         <v>42856</v>
       </c>
@@ -2429,7 +2621,7 @@
         <v>62.58000183105469</v>
       </c>
       <c r="F66">
-        <v>57.88219833374023</v>
+        <v>57.8821907043457</v>
       </c>
       <c r="G66">
         <v>86200</v>
@@ -2438,13 +2630,16 @@
         <v>0.05194150387301733</v>
       </c>
       <c r="I66">
-        <v>0.06828268820366445</v>
+        <v>0.04315798042276185</v>
       </c>
       <c r="J66">
         <v>0.06828268820366445</v>
       </c>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="K66">
+        <v>0.06828268820366445</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="2">
         <v>42887</v>
       </c>
@@ -2461,7 +2656,7 @@
         <v>62.66999816894531</v>
       </c>
       <c r="F67">
-        <v>58.70000076293945</v>
+        <v>58.69999313354492</v>
       </c>
       <c r="G67">
         <v>37800</v>
@@ -2470,13 +2665,16 @@
         <v>0.001438100595356095</v>
       </c>
       <c r="I67">
-        <v>0.1320447521315034</v>
+        <v>0.04285016267065887</v>
       </c>
       <c r="J67">
         <v>0.1320447521315034</v>
       </c>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="K67">
+        <v>0.1320447521315034</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="2">
         <v>42917</v>
       </c>
@@ -2502,13 +2700,16 @@
         <v>0.0507419881615947</v>
       </c>
       <c r="I68">
-        <v>0.1504192268200668</v>
+        <v>0.04275512675606971</v>
       </c>
       <c r="J68">
         <v>0.1504192268200668</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="K68">
+        <v>0.1504192268200668</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="2">
         <v>42948</v>
       </c>
@@ -2525,7 +2726,7 @@
         <v>67.70999908447266</v>
       </c>
       <c r="F69">
-        <v>63.42072296142578</v>
+        <v>63.42071914672852</v>
       </c>
       <c r="G69">
         <v>7300</v>
@@ -2534,13 +2735,16 @@
         <v>0.02824602359076045</v>
       </c>
       <c r="I69">
-        <v>0.2013839310008179</v>
+        <v>0.04246149181912138</v>
       </c>
       <c r="J69">
         <v>0.2013839310008179</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="K69">
+        <v>0.2013839310008179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="2">
         <v>42979</v>
       </c>
@@ -2566,13 +2770,16 @@
         <v>0.002953841092025344</v>
       </c>
       <c r="I70">
-        <v>0.2229426464066142</v>
+        <v>0.04216898594264727</v>
       </c>
       <c r="J70">
         <v>0.2229426464066142</v>
       </c>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="K70">
+        <v>0.2229426464066142</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="2">
         <v>43009</v>
       </c>
@@ -2589,7 +2796,7 @@
         <v>68.41999816894531</v>
       </c>
       <c r="F71">
-        <v>64.08575439453125</v>
+        <v>64.08574676513672</v>
       </c>
       <c r="G71">
         <v>8500</v>
@@ -2598,13 +2805,16 @@
         <v>0.007509858332116259</v>
       </c>
       <c r="I71">
-        <v>0.2941176385703059</v>
+        <v>0.04186717859021309</v>
       </c>
       <c r="J71">
         <v>0.2941176385703059</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="K71">
+        <v>0.2941176385703059</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="2">
         <v>43040</v>
       </c>
@@ -2621,7 +2831,7 @@
         <v>66.38999938964844</v>
       </c>
       <c r="F72">
-        <v>62.18434524536133</v>
+        <v>62.1843376159668</v>
       </c>
       <c r="G72">
         <v>23300</v>
@@ -2630,13 +2840,16 @@
         <v>-0.02966967017865629</v>
       </c>
       <c r="I72">
-        <v>0.3579464147775242</v>
+        <v>0.04190078481706322</v>
       </c>
       <c r="J72">
         <v>0.3579464147775242</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="K72">
+        <v>0.3579464147775242</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="2">
         <v>43070</v>
       </c>
@@ -2653,7 +2866,7 @@
         <v>67.58999633789062</v>
       </c>
       <c r="F73">
-        <v>63.85403823852539</v>
+        <v>63.85404968261719</v>
       </c>
       <c r="G73">
         <v>9200</v>
@@ -2662,13 +2875,16 @@
         <v>0.01807496549592225</v>
       </c>
       <c r="I73">
-        <v>0.3255539147478406</v>
+        <v>0.04160303796699926</v>
       </c>
       <c r="J73">
         <v>0.3255539147478406</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="K73">
+        <v>0.3255539147478406</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="2">
         <v>43101</v>
       </c>
@@ -2685,7 +2901,7 @@
         <v>69.72000122070312</v>
       </c>
       <c r="F74">
-        <v>65.86631774902344</v>
+        <v>65.86632537841797</v>
       </c>
       <c r="G74">
         <v>13600</v>
@@ -2694,13 +2910,16 @@
         <v>0.03151361145463527</v>
       </c>
       <c r="I74">
-        <v>0.293986633975061</v>
+        <v>0.04135940845291071</v>
       </c>
       <c r="J74">
         <v>0.293986633975061</v>
       </c>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="K74">
+        <v>0.293986633975061</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="2">
         <v>43132</v>
       </c>
@@ -2717,7 +2936,7 @@
         <v>68.23999786376953</v>
       </c>
       <c r="F75">
-        <v>64.46811676025391</v>
+        <v>64.46812438964844</v>
       </c>
       <c r="G75">
         <v>10300</v>
@@ -2726,13 +2945,16 @@
         <v>-0.02122781599283896</v>
       </c>
       <c r="I75">
-        <v>0.2750373183875892</v>
+        <v>0.04128275289730066</v>
       </c>
       <c r="J75">
         <v>0.2750373183875892</v>
       </c>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="K75">
+        <v>0.2750373183875892</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="2">
         <v>43160</v>
       </c>
@@ -2749,7 +2971,7 @@
         <v>68.69000244140625</v>
       </c>
       <c r="F76">
-        <v>64.89325714111328</v>
+        <v>64.89324951171875</v>
       </c>
       <c r="G76">
         <v>25800</v>
@@ -2758,13 +2980,16 @@
         <v>0.006594440089741527</v>
       </c>
       <c r="I76">
-        <v>0.2398917066693438</v>
+        <v>0.04100792859592801</v>
       </c>
       <c r="J76">
         <v>0.2398917066693438</v>
       </c>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="K76">
+        <v>0.2398917066693438</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="2">
         <v>43191</v>
       </c>
@@ -2781,7 +3006,7 @@
         <v>66.91999816894531</v>
       </c>
       <c r="F77">
-        <v>63.22109222412109</v>
+        <v>63.22108459472656</v>
       </c>
       <c r="G77">
         <v>57200</v>
@@ -2790,13 +3015,16 @@
         <v>-0.02576800421532643</v>
       </c>
       <c r="I77">
-        <v>0.1248948778088184</v>
+        <v>0.04098598503584924</v>
       </c>
       <c r="J77">
         <v>0.1248948778088184</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="K77">
+        <v>0.1248948778088184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="2">
         <v>43221</v>
       </c>
@@ -2813,7 +3041,7 @@
         <v>66.01999664306641</v>
       </c>
       <c r="F78">
-        <v>62.37082290649414</v>
+        <v>62.37082672119141</v>
       </c>
       <c r="G78">
         <v>11700</v>
@@ -2822,13 +3050,16 @@
         <v>-0.01344891737155718</v>
       </c>
       <c r="I78">
-        <v>0.05496955435218065</v>
+        <v>0.04082745967556214</v>
       </c>
       <c r="J78">
         <v>0.05496955435218065</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="K78">
+        <v>0.05496955435218065</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="2">
         <v>43252</v>
       </c>
@@ -2845,7 +3076,7 @@
         <v>63.88999938964844</v>
       </c>
       <c r="F79">
-        <v>61.21242904663086</v>
+        <v>61.21243286132812</v>
       </c>
       <c r="G79">
         <v>3600</v>
@@ -2854,13 +3085,16 @@
         <v>-0.03226291065923081</v>
       </c>
       <c r="I79">
-        <v>0.01946706967206624</v>
+        <v>0.04088419815453751</v>
       </c>
       <c r="J79">
         <v>0.01946706967206624</v>
       </c>
-    </row>
-    <row r="80" spans="1:10">
+      <c r="K79">
+        <v>0.01946706967206624</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="2">
         <v>43282</v>
       </c>
@@ -2886,13 +3120,16 @@
         <v>0.06229462192761326</v>
       </c>
       <c r="I80">
-        <v>0.03067584387651578</v>
+        <v>0.04100916093833593</v>
       </c>
       <c r="J80">
         <v>0.03067584387651578</v>
       </c>
-    </row>
-    <row r="81" spans="1:10">
+      <c r="K80">
+        <v>0.03067584387651578</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="2">
         <v>43313</v>
       </c>
@@ -2909,7 +3146,7 @@
         <v>67.59999847412109</v>
       </c>
       <c r="F81">
-        <v>64.76696014404297</v>
+        <v>64.76695251464844</v>
       </c>
       <c r="G81">
         <v>2900</v>
@@ -2918,13 +3155,16 @@
         <v>-0.003978256395083646</v>
       </c>
       <c r="I81">
-        <v>-0.001624584431234921</v>
+        <v>0.04079029180272387</v>
       </c>
       <c r="J81">
         <v>-0.001624584431234921</v>
       </c>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="K81">
+        <v>-0.001624584431234921</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="2">
         <v>43344</v>
       </c>
@@ -2941,7 +3181,7 @@
         <v>64.56999969482422</v>
       </c>
       <c r="F82">
-        <v>61.86393356323242</v>
+        <v>61.86392974853516</v>
       </c>
       <c r="G82">
         <v>21500</v>
@@ -2950,13 +3190,16 @@
         <v>-0.04482246816110258</v>
       </c>
       <c r="I82">
-        <v>-0.04918279763175337</v>
+        <v>0.04104020056588451</v>
       </c>
       <c r="J82">
         <v>-0.04918279763175337</v>
       </c>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="K82">
+        <v>-0.04918279763175337</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="2">
         <v>43374</v>
       </c>
@@ -2982,13 +3225,16 @@
         <v>-0.1025243760751544</v>
       </c>
       <c r="I83">
-        <v>-0.1530253973429367</v>
+        <v>0.04272478901161512</v>
       </c>
       <c r="J83">
         <v>-0.1530253973429367</v>
       </c>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="K83">
+        <v>-0.1530253973429367</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="2">
         <v>43405</v>
       </c>
@@ -3005,7 +3251,7 @@
         <v>58.41999816894531</v>
       </c>
       <c r="F84">
-        <v>55.9716682434082</v>
+        <v>55.97167205810547</v>
       </c>
       <c r="G84">
         <v>28700</v>
@@ -3014,13 +3260,16 @@
         <v>0.008110395165109807</v>
       </c>
       <c r="I84">
-        <v>-0.1200482195206318</v>
+        <v>0.04246117731021379</v>
       </c>
       <c r="J84">
         <v>-0.1200482195206318</v>
       </c>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="K84">
+        <v>-0.1200482195206318</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="2">
         <v>43435</v>
       </c>
@@ -3037,7 +3286,7 @@
         <v>56.81000137329102</v>
       </c>
       <c r="F85">
-        <v>54.63984680175781</v>
+        <v>54.63984298706055</v>
       </c>
       <c r="G85">
         <v>7300</v>
@@ -3046,13 +3295,16 @@
         <v>-0.02755900113174148</v>
       </c>
       <c r="I85">
-        <v>-0.159490983113967</v>
+        <v>0.04240923556696467</v>
       </c>
       <c r="J85">
         <v>-0.159490983113967</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="K85">
+        <v>-0.159490983113967</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="2">
         <v>43466</v>
       </c>
@@ -3069,7 +3321,7 @@
         <v>59.16999816894531</v>
       </c>
       <c r="F86">
-        <v>56.90969085693359</v>
+        <v>56.90968704223633</v>
       </c>
       <c r="G86">
         <v>51200</v>
@@ -3078,13 +3330,16 @@
         <v>0.04154192463659823</v>
       </c>
       <c r="I86">
-        <v>-0.151319605092391</v>
+        <v>0.04229166016487586</v>
       </c>
       <c r="J86">
         <v>-0.151319605092391</v>
       </c>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="K86">
+        <v>-0.151319605092391</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="2">
         <v>43497</v>
       </c>
@@ -3101,7 +3356,7 @@
         <v>62.08000183105469</v>
       </c>
       <c r="F87">
-        <v>59.70852661132812</v>
+        <v>59.70853042602539</v>
       </c>
       <c r="G87">
         <v>6400</v>
@@ -3110,13 +3365,16 @@
         <v>0.04918039128209162</v>
       </c>
       <c r="I87">
-        <v>-0.09026958126540852</v>
+        <v>0.04224744837682679</v>
       </c>
       <c r="J87">
         <v>-0.09026958126540852</v>
       </c>
-    </row>
-    <row r="88" spans="1:10">
+      <c r="K87">
+        <v>-0.09026958126540852</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="2">
         <v>43525</v>
       </c>
@@ -3133,7 +3391,7 @@
         <v>63.04999923706055</v>
       </c>
       <c r="F88">
-        <v>60.64147567749023</v>
+        <v>60.64147186279297</v>
       </c>
       <c r="G88">
         <v>2500</v>
@@ -3142,13 +3400,16 @@
         <v>0.01562495775444117</v>
       </c>
       <c r="I88">
-        <v>-0.08210806527713732</v>
+        <v>0.04200115191444728</v>
       </c>
       <c r="J88">
         <v>-0.08210806527713732</v>
       </c>
-    </row>
-    <row r="89" spans="1:10">
+      <c r="K88">
+        <v>-0.08210806527713732</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="2">
         <v>43556</v>
       </c>
@@ -3165,7 +3426,7 @@
         <v>64.29000091552734</v>
       </c>
       <c r="F89">
-        <v>61.83409881591797</v>
+        <v>61.83410263061523</v>
       </c>
       <c r="G89">
         <v>8300</v>
@@ -3174,13 +3435,16 @@
         <v>0.01966695786632022</v>
       </c>
       <c r="I89">
-        <v>-0.03930061753406378</v>
+        <v>0.04176644030321192</v>
       </c>
       <c r="J89">
         <v>-0.03930061753406378</v>
       </c>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="K89">
+        <v>-0.03930061753406378</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="2">
         <v>43586</v>
       </c>
@@ -3197,7 +3461,7 @@
         <v>61.16999816894531</v>
       </c>
       <c r="F90">
-        <v>58.83329010009766</v>
+        <v>58.83328628540039</v>
       </c>
       <c r="G90">
         <v>19100</v>
@@ -3206,13 +3470,16 @@
         <v>-0.0485301400241307</v>
       </c>
       <c r="I90">
-        <v>-0.07346256771781356</v>
+        <v>0.04201036190204152</v>
       </c>
       <c r="J90">
         <v>-0.07346256771781356</v>
       </c>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="K90">
+        <v>-0.07346256771781356</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="2">
         <v>43617</v>
       </c>
@@ -3229,7 +3496,7 @@
         <v>62.38000106811523</v>
       </c>
       <c r="F91">
-        <v>61.47555541992188</v>
+        <v>61.47555923461914</v>
       </c>
       <c r="G91">
         <v>700</v>
@@ -3238,13 +3505,16 @@
         <v>0.01978098635589332</v>
       </c>
       <c r="I91">
-        <v>-0.02363434553073196</v>
+        <v>0.04178261679215959</v>
       </c>
       <c r="J91">
         <v>-0.02363434553073196</v>
       </c>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="K91">
+        <v>-0.02363434553073196</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="2">
         <v>43647</v>
       </c>
@@ -3261,7 +3531,7 @@
         <v>60.09000015258789</v>
       </c>
       <c r="F92">
-        <v>59.2187614440918</v>
+        <v>59.21875762939453</v>
       </c>
       <c r="G92">
         <v>4700</v>
@@ -3270,13 +3540,16 @@
         <v>-0.03671049817756178</v>
       </c>
       <c r="I92">
-        <v>-0.1146309456188426</v>
+        <v>0.04184525655815156</v>
       </c>
       <c r="J92">
         <v>-0.1146309456188426</v>
       </c>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="K92">
+        <v>-0.1146309456188426</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="2">
         <v>43678</v>
       </c>
@@ -3293,7 +3566,7 @@
         <v>60.79999923706055</v>
       </c>
       <c r="F93">
-        <v>59.91846466064453</v>
+        <v>59.9184684753418</v>
       </c>
       <c r="G93">
         <v>10200</v>
@@ -3302,13 +3575,16 @@
         <v>0.01181559465251691</v>
       </c>
       <c r="I93">
-        <v>-0.1005917069608182</v>
+        <v>0.0416125407486674</v>
       </c>
       <c r="J93">
         <v>-0.1005917069608182</v>
       </c>
-    </row>
-    <row r="94" spans="1:10">
+      <c r="K93">
+        <v>-0.1005917069608182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="2">
         <v>43709</v>
       </c>
@@ -3334,13 +3610,16 @@
         <v>0.0004934637232010264</v>
       </c>
       <c r="I94">
-        <v>-0.05792160262421875</v>
+        <v>0.0413953332007754</v>
       </c>
       <c r="J94">
         <v>-0.05792160262421875</v>
       </c>
-    </row>
-    <row r="95" spans="1:10">
+      <c r="K94">
+        <v>-0.05792160262421875</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="2">
         <v>43739</v>
       </c>
@@ -3357,7 +3636,7 @@
         <v>62.72999954223633</v>
       </c>
       <c r="F95">
-        <v>61.82048034667969</v>
+        <v>61.82047653198242</v>
       </c>
       <c r="G95">
         <v>6000</v>
@@ -3366,13 +3645,16 @@
         <v>0.03123454962994354</v>
       </c>
       <c r="I95">
-        <v>0.08248487862581366</v>
+        <v>0.04122872639906538</v>
       </c>
       <c r="J95">
         <v>0.08248487862581366</v>
       </c>
-    </row>
-    <row r="96" spans="1:10">
+      <c r="K95">
+        <v>0.08248487862581366</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="2">
         <v>43770</v>
       </c>
@@ -3389,7 +3671,7 @@
         <v>65.26000213623047</v>
       </c>
       <c r="F96">
-        <v>64.31381225585938</v>
+        <v>64.31380462646484</v>
       </c>
       <c r="G96">
         <v>3000</v>
@@ -3398,13 +3680,16 @@
         <v>0.04033162143243252</v>
       </c>
       <c r="I96">
-        <v>0.1170832622675626</v>
+        <v>0.04112404412796106</v>
       </c>
       <c r="J96">
         <v>0.1170832622675626</v>
       </c>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="K96">
+        <v>0.1170832622675626</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="2">
         <v>43800</v>
       </c>
@@ -3421,7 +3706,7 @@
         <v>68.84999847412109</v>
       </c>
       <c r="F97">
-        <v>67.95657348632812</v>
+        <v>67.95658111572266</v>
       </c>
       <c r="G97">
         <v>11100</v>
@@ -3430,13 +3715,16 @@
         <v>0.05501066840905855</v>
       </c>
       <c r="I97">
-        <v>0.2119344624147577</v>
+        <v>0.04115857372442283</v>
       </c>
       <c r="J97">
         <v>0.2119344624147577</v>
       </c>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="K97">
+        <v>0.2119344624147577</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="2">
         <v>43831</v>
       </c>
@@ -3462,13 +3750,16 @@
         <v>0.00566447927802094</v>
       </c>
       <c r="I98">
-        <v>0.1701875951740242</v>
+        <v>0.04094498703834184</v>
       </c>
       <c r="J98">
         <v>0.1701875951740242</v>
       </c>
-    </row>
-    <row r="99" spans="1:10">
+      <c r="K98">
+        <v>0.1701875951740242</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="2">
         <v>43862</v>
       </c>
@@ -3494,13 +3785,16 @@
         <v>-0.05372618913163851</v>
       </c>
       <c r="I99">
-        <v>0.05541228593023195</v>
+        <v>0.04125693020161275</v>
       </c>
       <c r="J99">
         <v>0.05541228593023195</v>
       </c>
-    </row>
-    <row r="100" spans="1:10">
+      <c r="K99">
+        <v>0.05541228593023195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="2">
         <v>43891</v>
       </c>
@@ -3517,7 +3811,7 @@
         <v>60.06000137329102</v>
       </c>
       <c r="F100">
-        <v>59.28064346313477</v>
+        <v>59.2806396484375</v>
       </c>
       <c r="G100">
         <v>2200</v>
@@ -3526,13 +3820,16 @@
         <v>-0.08333326540780872</v>
       </c>
       <c r="I100">
-        <v>-0.04742264710468103</v>
+        <v>0.04211876100192706</v>
       </c>
       <c r="J100">
         <v>-0.04742264710468103</v>
       </c>
-    </row>
-    <row r="101" spans="1:10">
+      <c r="K100">
+        <v>-0.04742264710468103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="2">
         <v>43922</v>
       </c>
@@ -3549,7 +3846,7 @@
         <v>65.66999816894531</v>
       </c>
       <c r="F101">
-        <v>64.81784057617188</v>
+        <v>64.81784820556641</v>
       </c>
       <c r="G101">
         <v>5700</v>
@@ -3558,13 +3855,16 @@
         <v>0.09340653791841391</v>
       </c>
       <c r="I101">
-        <v>0.02146519262351831</v>
+        <v>0.04274712515805674</v>
       </c>
       <c r="J101">
         <v>0.02146519262351831</v>
       </c>
-    </row>
-    <row r="102" spans="1:10">
+      <c r="K101">
+        <v>0.02146519262351831</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="2">
         <v>43952</v>
       </c>
@@ -3590,13 +3890,16 @@
         <v>0.09760931690021879</v>
       </c>
       <c r="I102">
-        <v>0.1783554681819191</v>
+        <v>0.0434203358243174</v>
       </c>
       <c r="J102">
         <v>0.1783554681819191</v>
       </c>
-    </row>
-    <row r="103" spans="1:10">
+      <c r="K102">
+        <v>0.1783554681819191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="2">
         <v>43983</v>
       </c>
@@ -3622,13 +3925,16 @@
         <v>0.02219753653546319</v>
       </c>
       <c r="I103">
-        <v>0.1811477884510073</v>
+        <v>0.04321695500754568</v>
       </c>
       <c r="J103">
         <v>0.1811477884510073</v>
       </c>
-    </row>
-    <row r="104" spans="1:10">
+      <c r="K103">
+        <v>0.1811477884510073</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="2">
         <v>44013</v>
       </c>
@@ -3654,13 +3960,16 @@
         <v>0.08238327456138483</v>
       </c>
       <c r="I104">
-        <v>0.3271758994423204</v>
+        <v>0.04357707221968089</v>
       </c>
       <c r="J104">
         <v>0.3271758994423204</v>
       </c>
-    </row>
-    <row r="105" spans="1:10">
+      <c r="K104">
+        <v>0.3271758994423204</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="2">
         <v>44044</v>
       </c>
@@ -3686,13 +3995,16 @@
         <v>0.05291537580818972</v>
       </c>
       <c r="I105">
-        <v>0.3810855637234833</v>
+        <v>0.04355133143222953</v>
       </c>
       <c r="J105">
         <v>0.3810855637234833</v>
       </c>
-    </row>
-    <row r="106" spans="1:10">
+      <c r="K105">
+        <v>0.3810855637234833</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="2">
         <v>44075</v>
       </c>
@@ -3718,13 +4030,16 @@
         <v>0.008217249391156756</v>
       </c>
       <c r="I106">
-        <v>0.3917475113224325</v>
+        <v>0.04334120216923242</v>
       </c>
       <c r="J106">
         <v>0.3917475113224325</v>
       </c>
-    </row>
-    <row r="107" spans="1:10">
+      <c r="K106">
+        <v>0.3917475113224325</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="2">
         <v>44105</v>
       </c>
@@ -3741,7 +4056,7 @@
         <v>82.52999877929688</v>
       </c>
       <c r="F107">
-        <v>81.86833953857422</v>
+        <v>81.86833190917969</v>
       </c>
       <c r="G107">
         <v>12100</v>
@@ -3750,13 +4065,16 @@
         <v>-0.02515951796214966</v>
       </c>
       <c r="I107">
-        <v>0.3156384406432067</v>
+        <v>0.04328620653765526</v>
       </c>
       <c r="J107">
         <v>0.3156384406432067</v>
       </c>
-    </row>
-    <row r="108" spans="1:10">
+      <c r="K107">
+        <v>0.3156384406432067</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="2">
         <v>44136</v>
       </c>
@@ -3782,13 +4100,16 @@
         <v>0.1038410253433089</v>
       </c>
       <c r="I108">
-        <v>0.3959545738896781</v>
+        <v>0.04399638333526365</v>
       </c>
       <c r="J108">
         <v>0.3959545738896781</v>
       </c>
-    </row>
-    <row r="109" spans="1:10">
+      <c r="K108">
+        <v>0.3959545738896781</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="2">
         <v>44166</v>
       </c>
@@ -3814,13 +4135,16 @@
         <v>0.07145995878451927</v>
       </c>
       <c r="I109">
-        <v>0.4177197207497485</v>
+        <v>0.04415504335133285</v>
       </c>
       <c r="J109">
         <v>0.4177197207497485</v>
       </c>
-    </row>
-    <row r="110" spans="1:10">
+      <c r="K109">
+        <v>0.4177197207497485</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" s="2">
         <v>44197</v>
       </c>
@@ -3846,13 +4170,16 @@
         <v>-0.03995493803393446</v>
       </c>
       <c r="I110">
-        <v>0.3534084629645444</v>
+        <v>0.04424562728324995</v>
       </c>
       <c r="J110">
         <v>0.3534084629645444</v>
       </c>
-    </row>
-    <row r="111" spans="1:10">
+      <c r="K110">
+        <v>0.3534084629645444</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" s="2">
         <v>44228</v>
       </c>
@@ -3878,13 +4205,16 @@
         <v>0.006509450606244194</v>
       </c>
       <c r="I111">
-        <v>0.4395605086589325</v>
+        <v>0.04404439950519769</v>
       </c>
       <c r="J111">
         <v>0.4395605086589325</v>
       </c>
-    </row>
-    <row r="112" spans="1:10">
+      <c r="K111">
+        <v>0.4395605086589325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" s="2">
         <v>44256</v>
       </c>
@@ -3910,13 +4240,16 @@
         <v>0.02703565585250689</v>
       </c>
       <c r="I112">
-        <v>0.6128871217385721</v>
+        <v>0.04386314369852935</v>
       </c>
       <c r="J112">
         <v>0.6128871217385721</v>
       </c>
-    </row>
-    <row r="113" spans="1:10">
+      <c r="K112">
+        <v>0.6128871217385721</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" s="2">
         <v>44287</v>
       </c>
@@ -3942,13 +4275,16 @@
         <v>0.07009394779610378</v>
       </c>
       <c r="I113">
-        <v>0.5784986531510086</v>
+        <v>0.04400008951597798</v>
       </c>
       <c r="J113">
         <v>0.5784986531510086</v>
       </c>
-    </row>
-    <row r="114" spans="1:10">
+      <c r="K113">
+        <v>0.5784986531510086</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" s="2">
         <v>44317</v>
       </c>
@@ -3974,13 +4310,16 @@
         <v>0.04234998296891934</v>
       </c>
       <c r="I114">
-        <v>0.4990288610842673</v>
+        <v>0.04388699198943582</v>
       </c>
       <c r="J114">
         <v>0.4990288610842673</v>
       </c>
-    </row>
-    <row r="115" spans="1:10">
+      <c r="K114">
+        <v>0.4990288610842673</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" s="2">
         <v>44348</v>
       </c>
@@ -4006,13 +4345,16 @@
         <v>0.0006478453757257085</v>
       </c>
       <c r="I115">
-        <v>0.4674267412969453</v>
+        <v>0.04370767479023526</v>
       </c>
       <c r="J115">
         <v>0.4674267412969453</v>
       </c>
-    </row>
-    <row r="116" spans="1:10">
+      <c r="K115">
+        <v>0.4674267412969453</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" s="2">
         <v>44378</v>
       </c>
@@ -4038,13 +4380,16 @@
         <v>0.03718087810715942</v>
       </c>
       <c r="I116">
-        <v>0.406144192973648</v>
+        <v>0.04357029783367193</v>
       </c>
       <c r="J116">
         <v>0.406144192973648</v>
       </c>
-    </row>
-    <row r="117" spans="1:10">
+      <c r="K116">
+        <v>0.406144192973648</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="2">
         <v>44409</v>
       </c>
@@ -4070,13 +4415,16 @@
         <v>0.02541464677753669</v>
       </c>
       <c r="I117">
-        <v>0.3694176038122803</v>
+        <v>0.04339249514417814</v>
       </c>
       <c r="J117">
         <v>0.3694176038122803</v>
       </c>
-    </row>
-    <row r="118" spans="1:10">
+      <c r="K117">
+        <v>0.3694176038122803</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" s="2">
         <v>44440</v>
       </c>
@@ -4102,13 +4450,16 @@
         <v>-0.06687533659338074</v>
       </c>
       <c r="I118">
-        <v>0.2674226129260286</v>
+        <v>0.04384823195333051</v>
       </c>
       <c r="J118">
         <v>0.2674226129260286</v>
       </c>
-    </row>
-    <row r="119" spans="1:10">
+      <c r="K118">
+        <v>0.2674226129260286</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" s="2">
         <v>44470</v>
       </c>
@@ -4134,13 +4485,16 @@
         <v>0.06253493843085889</v>
       </c>
       <c r="I119">
-        <v>0.3814370995099363</v>
+        <v>0.04389717183669144</v>
       </c>
       <c r="J119">
         <v>0.3814370995099363</v>
       </c>
-    </row>
-    <row r="120" spans="1:10">
+      <c r="K119">
+        <v>0.3814370995099363</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" s="2">
         <v>44501</v>
       </c>
@@ -4166,42 +4520,83 @@
         <v>-0.06341551812528223</v>
       </c>
       <c r="I120">
-        <v>0.1721185572756077</v>
+        <v>0.04427962184936689</v>
       </c>
       <c r="J120">
         <v>0.1721185572756077</v>
       </c>
-    </row>
-    <row r="121" spans="1:10">
+      <c r="K120">
+        <v>0.1721185572756077</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" s="2">
         <v>44531</v>
       </c>
       <c r="B121">
-        <v>111.1080017089844</v>
+        <v>111.3300018310547</v>
       </c>
       <c r="C121">
-        <v>111.3099975585938</v>
+        <v>111.6600036621094</v>
       </c>
       <c r="D121">
-        <v>110.9400024414062</v>
+        <v>111.1699981689453</v>
       </c>
       <c r="E121">
-        <v>111.0100021362305</v>
+        <v>111.2200012207031</v>
       </c>
       <c r="F121">
-        <v>111.0100021362305</v>
+        <v>111.2200012207031</v>
       </c>
       <c r="G121">
-        <v>12863</v>
+        <v>5300</v>
       </c>
       <c r="H121">
-        <v>0.03961419184576487</v>
+        <v>0.04158084371758863</v>
       </c>
       <c r="I121">
-        <v>0.1372810310633052</v>
+        <v>0.04416996045989754</v>
       </c>
       <c r="J121">
-        <v>0.1372810310633052</v>
+        <v>0.139432440582407</v>
+      </c>
+      <c r="K121">
+        <v>0.139432440582407</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="2">
+        <v>44562</v>
+      </c>
+      <c r="B122">
+        <v>111.120002746582</v>
+      </c>
+      <c r="C122">
+        <v>111.120002746582</v>
+      </c>
+      <c r="D122">
+        <v>110.4595031738281</v>
+      </c>
+      <c r="E122">
+        <v>110.6600036621094</v>
+      </c>
+      <c r="F122">
+        <v>110.6600036621094</v>
+      </c>
+      <c r="G122">
+        <v>23462</v>
+      </c>
+      <c r="H122">
+        <v>-0.00503504362927043</v>
+      </c>
+      <c r="I122">
+        <v>0.04401523818011051</v>
+      </c>
+      <c r="J122">
+        <v>0.1808772248771184</v>
+      </c>
+      <c r="K122">
+        <v>0.1808772248771184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>